<commit_message>
Final version of Process Hierarchy template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-process-hierarchy/SAP Cloud ALM - Process Hierarchy template.xlsx
+++ b/spreadsheet-examples/spreadsheet-process-hierarchy/SAP Cloud ALM - Process Hierarchy template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d055585/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E7F38B-953A-DC4E-85D8-8736ACCBCB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2C8977-0892-D244-9EAE-568EE98F6E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="35840" windowHeight="21880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data example" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -60,42 +60,6 @@
     <t>External Reference URL</t>
   </si>
   <si>
-    <t>"External Reference URL" (optional) is used to indicate the URL for navigating to the Process Hierarchy node in the system specified by "External Reference Name". This property can only be indicated if "External Reference Name" and "External Reference ID" were provided for the Process Hierarchy node. Example: "https://mysapsolutionmanager.mycompany.com/cFAp0oqp7jsMrwlvSbxPaG".</t>
-  </si>
-  <si>
-    <t>The properties (columns) for which values can be provided for each Process Hierarchy node are:</t>
-  </si>
-  <si>
-    <t>The first row acts as header. The header names are used by SAP Cloud ALM to identify which property of the Process Hierarchy corresponds to which column in the spreadsheet.</t>
-  </si>
-  <si>
-    <t>The first sheet contains the data of the Process Hierarchy nodes to be uploaded. All other sheets are ignored.</t>
-  </si>
-  <si>
-    <t>The columns "External Reference Name" and "External Reference ID" (both optional) can be used for indicating that the Process Hierarchy node originates from or exists in another system. They specify the reference to it. They are always used together: Either both or none are filled for a Process Hierarchy node. Each combination of "External Reference Name" and "External Reference ID" must be unique. The combination of "External Reference Name" and "External Reference ID" is used by SAP Cloud ALM for identifying whether a node already exists in the Process Hierarchy.
-The "External Reference Name" indicates the system where the Process Hierarchy node also exsists. Any value (maximum 255 characters) can be specified. Example: "SAP Solution Manager".
-The "External Reference ID" indicates the ID of the Process Hierarchy node in the system. Any value (maximum 255 characters) can be specified. Example: "cFAp0oqp7jsMrwlvSbxPaG".
-The above example indicates that the Process Hierarchy node exists in system "SAP Solution Manager", where it has the ID "cFAp0oqp7jsMrwlvSbxPaG".</t>
-  </si>
-  <si>
-    <t>Each subsequent row represents a node of the Process Hierachy to be uploaded. A maximum of 10.000 rows are supported.</t>
-  </si>
-  <si>
-    <t>"Title" (mandatory): Indicates the title of the Process Hierarchy node, with a maximum length of 60 characters.</t>
-  </si>
-  <si>
-    <t>"Description" (optional): Indicates the description (plain text) of the Process Hierarchy node, with a maximum length of 2500 characters.</t>
-  </si>
-  <si>
-    <t>"Hierarchy" (mandatory): Indicates the parent/child relations between the Process Hierarchy nodes in the spreadsheet, as well as the sequence (order) of the nodes within each level of the hierarchy. The specified values must be unique. No gaps between values are allowed. A maximum depth of 10 hierarchy levels is allowed.
-Examples:
-    - The value 1 indicates that the node is a root node of the Process Hierarchy and it occupies the first position among the nodes provided in the spreadsheet.
-    - The value 2 indicates that the node is a root node of the Process Hierarchy and it occupies the second position among the nodes provided in the spreadsheet.
-    - The value 2.1 indicates that the node is the first child of the node having value "2" in the "Hierarchy" column.
-    - The value 2.3 indicates that the node is the third child of the node having value "2" in the "Hierarchy" column.
-    - The value 1.2.4 indicates that the node is the fourth child of the node having value "1.2" in the "Hierarchy" column.</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
@@ -205,6 +169,9 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>SAP Help Portal</t>
   </si>
 </sst>
 </file>
@@ -353,8 +320,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -542,7 +510,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,7 +631,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -706,12 +674,10 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -721,23 +687,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -771,6 +726,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1093,184 +1049,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11" style="2"/>
+    <col min="1" max="1" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="136" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1284,73 +1240,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66B9978-02C6-F042-A244-43B37724FB95}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C2131A-AA06-5646-A049-8A241B51003E}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="170.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="117.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="8"/>
-    </row>
-    <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="8"/>
-    </row>
-    <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="40" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="280" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="80" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
-        <v>8</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{DDC365B9-BA7E-7E4C-B5A4-E00B1F57533C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>